<commit_message>
update the excel file
</commit_message>
<xml_diff>
--- a/NeoCortexApi/NeoCortexApi.Experiments/SpatialSimilarityIndividualProjectJayashreeRegoti/Input And Output Values/potentialIndipendent.xlsx
+++ b/NeoCortexApi/NeoCortexApi.Experiments/SpatialSimilarityIndividualProjectJayashreeRegoti/Input And Output Values/potentialIndipendent.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayashree Regoti\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\neocortexapi\NeoCortexApi\NeoCortexApi.Experiments\SpatialSimilarityIndividualProjectJayashreeRegoti\Input And Output Values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1319CED-7178-4E39-8AED-A6C5CF5C5C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704FD5AD-580A-4D43-936A-52D9CDE4D3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{62D0615D-2408-4A09-BA66-97A5306EE16F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="9" xr2:uid="{62D0615D-2408-4A09-BA66-97A5306EE16F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="40">
   <si>
     <t>I-00</t>
   </si>
@@ -95,15 +95,91 @@
   <si>
     <t>r =045</t>
   </si>
+  <si>
+    <t>Input = comparing the simiarility of I-00 inout with other images inout</t>
+  </si>
+  <si>
+    <t>Similarly , I-03 = 15% , I-04 = 25%, I-05 = 35%, I-06 =50%, I-07 = 65%, I-08 =80%, I-09 =90%</t>
+  </si>
+  <si>
+    <t>where,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I-00 is first input image with 5% non-zero bits, I-02 is second input image with 10% non-zero bits,</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-01 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-01 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-00 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-02 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-02 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-03 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-03 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-04 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-04 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-05 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-05 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-06 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-06 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-07 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-07 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-08 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-08 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
+  <si>
+    <t>Input = comparing the simiarility of I-09 inout with other images inout</t>
+  </si>
+  <si>
+    <t>column 'r' = comparision of SDR of image I-09 with othe images SDR at at Potential radius 45, 56, 67, 90,101</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,8 +205,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16655,10 +16734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6FD2EA-B1B8-4D6B-BDF4-AA19A69FA062}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16921,18 +17000,42 @@
         <v>30.76</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3A732F-741B-4F87-A674-C164A41A3661}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17193,6 +17296,29 @@
       </c>
       <c r="G14">
         <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -17203,10 +17329,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3B5BDC-AC18-43A4-BBB0-41A316FA915B}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+    <sheetView topLeftCell="A3" zoomScale="94" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17467,6 +17593,29 @@
       </c>
       <c r="G14">
         <v>30.18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -17477,10 +17626,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F5FEBA-FC87-4836-B06E-D815D2ED56FC}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17741,6 +17890,29 @@
       </c>
       <c r="G14">
         <v>35.64</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -17751,10 +17923,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30A353-0F65-447F-A348-9CF3A4385FB9}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18015,6 +18187,29 @@
       </c>
       <c r="G14">
         <v>36.520000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -18025,10 +18220,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9B4EC9-52FE-4FF1-B9CD-480458272AB8}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18289,6 +18484,29 @@
       </c>
       <c r="G14">
         <v>39.06</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -18299,10 +18517,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB7D966-6835-4D4B-BDE0-F60B2B234CD5}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18563,6 +18781,29 @@
       </c>
       <c r="G14">
         <v>54.3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -18573,10 +18814,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C00D3C-C2B0-4958-9340-DDAEB1F906A6}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18837,6 +19078,29 @@
       </c>
       <c r="G14">
         <v>65.14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -18847,10 +19111,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBD250B-411C-43E0-AB04-9AEEF648D5A6}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19111,6 +19375,29 @@
       </c>
       <c r="G14">
         <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -19121,10 +19408,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAA9BB1-C4EE-4F4A-B325-2688742AF4C6}">
-  <dimension ref="A3:G14"/>
+  <dimension ref="A3:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19387,6 +19674,29 @@
         <v>91.31</v>
       </c>
     </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>